<commit_message>
general update + webscraping to find valid files from reddprojectdatabase
</commit_message>
<xml_diff>
--- a/verra.xlsx
+++ b/verra.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/epr26_cam_ac_uk/Documents/Post_Project_Permanence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="8_{901FC455-6756-4CDB-A0F3-7EBE46732636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69D2E422-814F-4A81-8ECC-0EBF4DFE9E19}"/>
+  <xr:revisionPtr revIDLastSave="373" documentId="8_{901FC455-6756-4CDB-A0F3-7EBE46732636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8DA5BFB-1594-439E-96DC-E0553BDE06A1}"/>
   <bookViews>
-    <workbookView xWindow="19960" yWindow="760" windowWidth="16810" windowHeight="15370" xr2:uid="{5C00AD7D-F780-4E33-866F-2E3F21760DB3}"/>
+    <workbookView xWindow="21970" yWindow="730" windowWidth="32950" windowHeight="16950" xr2:uid="{5C00AD7D-F780-4E33-866F-2E3F21760DB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>date_start</t>
   </si>
@@ -182,9 +182,6 @@
     <t>details</t>
   </si>
   <si>
-    <t>requested by PP on 2022/10/21, cited reasons being that it took too much time to issue credit and they were prevented from implementing other activities, and so they decided to registrate with another certification</t>
-  </si>
-  <si>
     <t>since 2022/04/11 due to legal concerns (but validation report published 2022/11/04?); a lot of things to correct during the VV process (news report: https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/energy-transition/041422-indonesia-halts-carbon-project-verification-process-over-legal-concerns</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>on hold for VCS, under validation for CCB</t>
   </si>
   <si>
-    <t>verification request denied by Verra in 2023/02/27; in report in 2010/07/12, comments 2-6 raise concerns over poor project design, local land dispute and consultation and lack of governmental support (PNG government disavows it) (VCU nevertheless issued in 2018?)</t>
-  </si>
-  <si>
     <t>reason not given; why is PP in India?</t>
   </si>
   <si>
@@ -245,13 +239,35 @@
     <t>polygon</t>
   </si>
   <si>
-    <t>reason not given; on 2020/11/03 status in reddprojectsdatabase.org is "standard 1 certification in process"; an 2022/10/14 pre-feasibility report exists, so withdrawal could be after that</t>
-  </si>
-  <si>
     <t>image&gt;shp</t>
   </si>
   <si>
-    <t>documents can be found at: https://www.climate-standards.org/2011/11/17/makira-protected-forest-area-project ; date_start is registration date; its mention on redd-monitor.org in an article on 2019/06/14 doesn't mention that it's failed, meaning the failure probably happened after that</t>
+    <t>date_end</t>
+  </si>
+  <si>
+    <t>reason not given;
+assume it happened in 2022?</t>
+  </si>
+  <si>
+    <t>withdrawal requested by PP on 21st Oct 2022, citing reasons as it taking too much time to issue credit, preventing them from implementing other activities, and so they decided to registrate with another certification (https://registry.verra.org/mymodule/ProjectDoc/Project_ViewFile.asp?FileID=80380&amp;IDKEY=s097809fdslkjf09rndasfufd098asodfjlkduf09nm23mrn87s110844020);
+end date is 21st Oct 2022 but it doesn't mean project actually stopped: could serve as control</t>
+  </si>
+  <si>
+    <t>PD at https://www.climate-standards.org/2011/11/17/makira-protected-forest-area-project;
+mentioned on redd-monitor.org on 2019/06/14, but no mention that it's failed (https://redd-monitor.org/2019/06/14/how-many-successful-redd-projects-are-there-verra-claims-more-than-150-but-the-reality-is-only-32-according-to-verras-own-project-database/);
+status in reddprojectdatabase on 17th Sep 2020 is "ongoing" (https://www.reddprojectsdatabase.org/view/project.php?id=407), meaning the failure probably happened after that; project registered on 13th Dec 2014, and validation report on 28th Sep 2012 (https://registry.verra.org/mymodule/ProjectDoc/Project_ViewFile.asp?FileID=37061&amp;IDKEY=9kjalskjf098234kj28098sfkjlf098098kl32lasjdflkj909251107119), which mentions "sufficient issues remained with several NCRs, which prevented prevent validation from occurring upon issuance of the final report. In general there is a lack of evidence to support or justify many important assertions made in the PD v3, however these will likely be addressed in v4 of the PD";
+assume it's 1st Jan 2021?</t>
+  </si>
+  <si>
+    <t>first period ends on 21st May 2019; 2nd verification request denied by Verra in 27th Feb 2023; reports in 12th Jul 2010 pointed out issues with poor project design, local land dispute and consultation and lack of governmental support (PNG government disavows it);
+assume that after the first period ended (21st May 2019), outside support significantly decreases?</t>
+  </si>
+  <si>
+    <t>reason not given;
+status in reddprojectsdatabase.org on 11th Mar 2020 is "standard 1 certification in process" (https://www.reddprojectsdatabase.org/view/project.php?id=862);
+a pre-feasibility report on 14th Oct 2022 pointed out issues with need to "clarify this situation between the Indigenous Reserve and the
+pertinent entities" and lack of legal certainty about the delimitation (https://pdf.usaid.gov/pdf_docs/PA00ZSF7.pdf), so withdrawal could be after that;
+assume it's 1st Jan 2023</t>
   </si>
 </sst>
 </file>
@@ -295,11 +311,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B62A697-79A9-4FE4-98FE-765AE02C04A5}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,16 +654,17 @@
     <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.81640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="225.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="137" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -661,28 +684,31 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
-        <v>67</v>
-      </c>
       <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>2262</v>
       </c>
@@ -701,29 +727,32 @@
       <c r="F2" s="3">
         <v>43908</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
+        <v>44927</v>
+      </c>
+      <c r="H2" s="2">
         <v>124923</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>30</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>3478764</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N2" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2872</v>
       </c>
@@ -742,70 +771,76 @@
       <c r="F3" s="3">
         <v>44560</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
+        <v>44742</v>
+      </c>
+      <c r="H3" s="2">
         <v>1260222</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>30</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>922896</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>2251</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>42736</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44012</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44855</v>
+      </c>
+      <c r="H4" s="2">
+        <v>809664</v>
+      </c>
+      <c r="I4" s="2">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2">
+        <v>438730</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2251</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>42736</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44012</v>
-      </c>
-      <c r="G4">
-        <v>809664</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-      <c r="I4">
-        <v>438730</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1175</v>
       </c>
@@ -824,58 +859,62 @@
       <c r="F5" s="1">
         <v>41734</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1"/>
+      <c r="H5">
         <v>50251</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>20</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>58154</v>
       </c>
-      <c r="K5" t="s">
-        <v>69</v>
-      </c>
       <c r="L5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6">
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>2177</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1">
-        <v>41683</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3">
+        <v>38353</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44197</v>
+      </c>
+      <c r="H6" s="2">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>1122</v>
       </c>
@@ -894,25 +933,28 @@
       <c r="F7" s="3">
         <v>41309</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
+        <v>43606</v>
+      </c>
+      <c r="H7">
         <v>196703</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3700</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -924,33 +966,33 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8">
+        <v>62</v>
+      </c>
+      <c r="H8">
         <v>181681</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>19</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>234910</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>14</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="M8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3690</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -962,33 +1004,34 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9">
+        <v>62</v>
+      </c>
+      <c r="H9">
         <v>814948</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>20</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1067300</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>14</v>
       </c>
-      <c r="L9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M9" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2320</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1">
         <v>42913</v>
@@ -999,26 +1042,27 @@
       <c r="F10" s="1">
         <v>44396</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1"/>
+      <c r="H10">
         <v>72010950</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>100</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>999999999</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>10</v>
       </c>
-      <c r="L10" t="s">
-        <v>60</v>
-      </c>
       <c r="M10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1434</v>
       </c>
@@ -1037,29 +1081,30 @@
       <c r="F11" s="1">
         <v>42035</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1"/>
+      <c r="H11">
         <v>681</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>100</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1781</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>22</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>14</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>44</v>
       </c>
-      <c r="M11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="N11" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2403</v>
       </c>
@@ -1078,34 +1123,35 @@
       <c r="F12" s="1">
         <v>44869</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1"/>
+      <c r="H12">
         <v>130090</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>57</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>6870411</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>18</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>10</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>35</v>
       </c>
-      <c r="M12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="N12" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2010</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -1119,29 +1165,30 @@
       <c r="F13" s="1">
         <v>43788</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1"/>
+      <c r="H13" t="s">
         <v>15</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>30</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>266253</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>18</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>14</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>44</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2420</v>
       </c>
@@ -1160,29 +1207,30 @@
       <c r="F14" s="1">
         <v>44219</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1"/>
+      <c r="H14">
         <v>11389</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>20</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>88964</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>18</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>10</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2419</v>
       </c>
@@ -1199,25 +1247,26 @@
         <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15">
+        <v>62</v>
+      </c>
+      <c r="H15">
         <v>9896</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>20</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>18</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>14</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2374</v>
       </c>
@@ -1236,34 +1285,35 @@
       <c r="F16" s="1">
         <v>44134</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1"/>
+      <c r="H16">
         <v>14197</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>60</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>435091</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>18</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>10</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>41</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1150</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
@@ -1272,27 +1322,120 @@
         <v>40147</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17">
+        <v>62</v>
+      </c>
+      <c r="I17">
         <v>20</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>14</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>44</v>
       </c>
-      <c r="M17" t="s">
-        <v>55</v>
-      </c>
+      <c r="N17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N31" s="5"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N32" s="5"/>
+    </row>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N33" s="5"/>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N34" s="5"/>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N35" s="5"/>
+    </row>
+    <row r="36" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N36" s="5"/>
+    </row>
+    <row r="37" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N37" s="5"/>
+    </row>
+    <row r="38" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N38" s="5"/>
+    </row>
+    <row r="39" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N39" s="5"/>
+    </row>
+    <row r="40" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N40" s="5"/>
+    </row>
+    <row r="41" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N41" s="5"/>
+    </row>
+    <row r="42" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N42" s="5"/>
+    </row>
+    <row r="43" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N43" s="5"/>
+    </row>
+    <row r="44" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N44" s="5"/>
+    </row>
+    <row r="45" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N45" s="5"/>
+    </row>
+    <row r="46" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N46" s="5"/>
+    </row>
+    <row r="47" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N47" s="5"/>
+    </row>
+    <row r="48" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N48" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M17" xr:uid="{0B62A697-79A9-4FE4-98FE-765AE02C04A5}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M17">
+  <autoFilter ref="A1:N17" xr:uid="{0B62A697-79A9-4FE4-98FE-765AE02C04A5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N17">
       <sortCondition descending="1" ref="E1:E17"/>
     </sortState>
   </autoFilter>

</xml_diff>